<commit_message>
Mejorando Interfaz y resultados
</commit_message>
<xml_diff>
--- a/Archivos/Resultados.xlsx
+++ b/Archivos/Resultados.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\El Proyecto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP\Documents\El Proyecto\Archivos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C881372B-E5A0-43C1-BA85-B288BEF591FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9BA22501-353A-4B8C-ADFF-10A4B61467B2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FA68BC49-A0B4-45D9-976E-79E5F52D2F97}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{FA68BC49-A0B4-45D9-976E-79E5F52D2F97}"/>
   </bookViews>
   <sheets>
     <sheet name="V1" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="213" uniqueCount="57">
   <si>
     <t>Casa</t>
   </si>
@@ -211,6 +211,9 @@
   </si>
   <si>
     <t>RESULTADOS DEL PROGRAMA VERSION 1</t>
+  </si>
+  <si>
+    <t>15 pts diferencia</t>
   </si>
 </sst>
 </file>
@@ -361,47 +364,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="54">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="6" tint="-0.24994659260841701"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="50">
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -689,13 +652,6 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color rgb="FF000000"/>
-        </bottom>
-      </border>
     </dxf>
     <dxf>
       <border outline="0">
@@ -733,244 +689,244 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color auto="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.749992370372631"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color rgb="FF000000"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.89999084444715716"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.89999084444715716"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.89999084444715716"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.89999084444715716"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.89999084444715716"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.89999084444715716"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <border outline="0">
         <bottom style="thin">
           <color rgb="FF000000"/>
         </bottom>
       </border>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color auto="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.749992370372631"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color rgb="FF000000"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1008,6 +964,13 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color rgb="FF000000"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1034,6 +997,63 @@
     </dxf>
     <dxf>
       <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
         <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
@@ -1060,7 +1080,7 @@
     <dxf>
       <font>
         <b val="0"/>
-        <i val="0"/>
+        <i/>
         <strike val="0"/>
         <condense val="0"/>
         <extend val="0"/>
@@ -1134,7 +1154,7 @@
     </dxf>
     <dxf>
       <font>
-        <b/>
+        <b val="0"/>
         <i val="0"/>
         <strike val="0"/>
         <condense val="0"/>
@@ -1149,7 +1169,6 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -1159,11 +1178,30 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <border outline="0">
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="1"/>
+        <name val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="19" formatCode="dd/mm/yyyy"/>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.89999084444715716"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <border outline="0">
@@ -1201,6 +1239,13 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <border outline="0">
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -1223,88 +1268,6 @@
           <bgColor theme="3" tint="0.749992370372631"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.89999084444715716"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -1321,14 +1284,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF5D3335-C203-414C-B5A4-B1AE54BC46BD}" name="Tabla2" displayName="Tabla2" ref="A2:F26" totalsRowShown="0" headerRowDxfId="48" dataDxfId="47" headerRowBorderDxfId="45" tableBorderDxfId="46">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{EF5D3335-C203-414C-B5A4-B1AE54BC46BD}" name="Tabla2" displayName="Tabla2" ref="A2:F26" totalsRowShown="0" headerRowDxfId="49" dataDxfId="47" headerRowBorderDxfId="48" tableBorderDxfId="46">
   <autoFilter ref="A2:F26" xr:uid="{EF5D3335-C203-414C-B5A4-B1AE54BC46BD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{0E447FFE-76DF-40D6-9B41-5A9BD26FD310}" name="Fecha" dataDxfId="44"/>
-    <tableColumn id="2" xr3:uid="{DE6DE503-5A73-4772-8C8C-CA7907C32390}" name="Casa" dataDxfId="43"/>
-    <tableColumn id="3" xr3:uid="{A1100241-296B-4835-A91E-5F599728700C}" name="Visitante" dataDxfId="42"/>
-    <tableColumn id="4" xr3:uid="{DFF2B1DE-CB62-4759-A466-8869F8A4603D}" name="Programa" dataDxfId="41"/>
-    <tableColumn id="5" xr3:uid="{ADEE255F-5BE1-4631-A79B-1A9E0D02464B}" name="Final" dataDxfId="49"/>
+    <tableColumn id="1" xr3:uid="{0E447FFE-76DF-40D6-9B41-5A9BD26FD310}" name="Fecha" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{DE6DE503-5A73-4772-8C8C-CA7907C32390}" name="Casa" dataDxfId="44"/>
+    <tableColumn id="3" xr3:uid="{A1100241-296B-4835-A91E-5F599728700C}" name="Visitante" dataDxfId="43"/>
+    <tableColumn id="4" xr3:uid="{DFF2B1DE-CB62-4759-A466-8869F8A4603D}" name="Programa" dataDxfId="42"/>
+    <tableColumn id="5" xr3:uid="{ADEE255F-5BE1-4631-A79B-1A9E0D02464B}" name="Final" dataDxfId="41"/>
     <tableColumn id="6" xr3:uid="{BEA2283A-F61D-4F27-A96F-4F954E19EEF6}" name="Observaciones" dataDxfId="40"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -1336,63 +1299,63 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{60AA24C5-54DC-462B-8486-C4D0E7EF0011}" name="Tabla5" displayName="Tabla5" ref="H1:I6" totalsRowShown="0" headerRowDxfId="53" dataDxfId="52">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{60AA24C5-54DC-462B-8486-C4D0E7EF0011}" name="Tabla5" displayName="Tabla5" ref="H1:I6" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38">
   <autoFilter ref="H1:I6" xr:uid="{60AA24C5-54DC-462B-8486-C4D0E7EF0011}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{317187C3-9528-48F3-B777-DFE0F873CB95}" name="Observación" dataDxfId="51"/>
-    <tableColumn id="2" xr3:uid="{5A989131-6717-49C3-9A42-6F8666D11AEC}" name="Descripción" dataDxfId="50"/>
+    <tableColumn id="1" xr3:uid="{317187C3-9528-48F3-B777-DFE0F873CB95}" name="Observación" dataDxfId="37"/>
+    <tableColumn id="2" xr3:uid="{5A989131-6717-49C3-9A42-6F8666D11AEC}" name="Descripción" dataDxfId="36"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0478C70F-FC27-490B-ADC8-30673CDC2762}" name="Tabla22" displayName="Tabla22" ref="A2:F26" totalsRowShown="0" headerRowDxfId="39" dataDxfId="38" headerRowBorderDxfId="36" tableBorderDxfId="37">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0478C70F-FC27-490B-ADC8-30673CDC2762}" name="Tabla22" displayName="Tabla22" ref="A2:F26" totalsRowShown="0" headerRowDxfId="35" dataDxfId="33" headerRowBorderDxfId="34" tableBorderDxfId="32">
   <autoFilter ref="A2:F26" xr:uid="{EF5D3335-C203-414C-B5A4-B1AE54BC46BD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{7D0592AF-3FAF-4799-BEE4-1DD6CD0925E6}" name="Fecha" dataDxfId="35"/>
-    <tableColumn id="2" xr3:uid="{35082669-5F77-4893-884D-C72D5BFE9650}" name="Casa" dataDxfId="34"/>
-    <tableColumn id="3" xr3:uid="{3B0A703D-AB03-4024-8595-4F35EE38B70A}" name="Visitante" dataDxfId="33"/>
-    <tableColumn id="4" xr3:uid="{7D3BC793-EB8A-4AE0-A37C-644E9A7FCF7B}" name="Programa" dataDxfId="32"/>
-    <tableColumn id="5" xr3:uid="{C5487BEB-B7F2-48C8-A8DA-09CAC14834E3}" name="Final" dataDxfId="31"/>
-    <tableColumn id="6" xr3:uid="{4ED31CB6-E146-4F6D-8251-11D3E337C189}" name="Observaciones" dataDxfId="30"/>
+    <tableColumn id="1" xr3:uid="{7D0592AF-3FAF-4799-BEE4-1DD6CD0925E6}" name="Fecha" dataDxfId="31"/>
+    <tableColumn id="2" xr3:uid="{35082669-5F77-4893-884D-C72D5BFE9650}" name="Casa" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{3B0A703D-AB03-4024-8595-4F35EE38B70A}" name="Visitante" dataDxfId="29"/>
+    <tableColumn id="4" xr3:uid="{7D3BC793-EB8A-4AE0-A37C-644E9A7FCF7B}" name="Programa" dataDxfId="28"/>
+    <tableColumn id="5" xr3:uid="{C5487BEB-B7F2-48C8-A8DA-09CAC14834E3}" name="Final" dataDxfId="27"/>
+    <tableColumn id="6" xr3:uid="{4ED31CB6-E146-4F6D-8251-11D3E337C189}" name="Observaciones" dataDxfId="26"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0012C3FD-6397-49F0-8750-74518696A024}" name="Tabla54" displayName="Tabla54" ref="H1:I6" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{0012C3FD-6397-49F0-8750-74518696A024}" name="Tabla54" displayName="Tabla54" ref="H1:I6" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24">
   <autoFilter ref="H1:I6" xr:uid="{60AA24C5-54DC-462B-8486-C4D0E7EF0011}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{F2F71751-E10F-4633-8CF4-61B2415126CA}" name="Observación" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{2061FD4D-E910-42A3-92F4-B58A119A98AD}" name="Descripción" dataDxfId="26"/>
+    <tableColumn id="1" xr3:uid="{F2F71751-E10F-4633-8CF4-61B2415126CA}" name="Observación" dataDxfId="23"/>
+    <tableColumn id="2" xr3:uid="{2061FD4D-E910-42A3-92F4-B58A119A98AD}" name="Descripción" dataDxfId="22"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9D12FC1F-9B18-4DCC-A6D2-D3619326812D}" name="Tabla225" displayName="Tabla225" ref="A2:F26" totalsRowShown="0" headerRowDxfId="25" dataDxfId="24" headerRowBorderDxfId="22" tableBorderDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{9D12FC1F-9B18-4DCC-A6D2-D3619326812D}" name="Tabla225" displayName="Tabla225" ref="A2:F26" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
   <autoFilter ref="A2:F26" xr:uid="{EF5D3335-C203-414C-B5A4-B1AE54BC46BD}"/>
   <tableColumns count="6">
-    <tableColumn id="1" xr3:uid="{23CC116F-E481-4509-BD18-30F166220288}" name="Fecha" dataDxfId="21"/>
-    <tableColumn id="2" xr3:uid="{6A3198C5-E092-4C16-803C-CC86B39579AB}" name="Casa" dataDxfId="20"/>
-    <tableColumn id="3" xr3:uid="{635A1EAB-821A-4F26-9065-6FB417518A06}" name="Visitante" dataDxfId="19"/>
-    <tableColumn id="4" xr3:uid="{FBE8146B-C7EC-4C50-B019-1EA1BA1BF381}" name="Programa" dataDxfId="18"/>
-    <tableColumn id="5" xr3:uid="{39A7C7D3-ADD2-468E-A2C2-BCC114E3E9AA}" name="Final" dataDxfId="17"/>
-    <tableColumn id="6" xr3:uid="{FDB540FF-D930-46F9-BFEA-73BA9AC35CE9}" name="Observaciones" dataDxfId="16"/>
+    <tableColumn id="1" xr3:uid="{23CC116F-E481-4509-BD18-30F166220288}" name="Fecha" dataDxfId="17"/>
+    <tableColumn id="2" xr3:uid="{6A3198C5-E092-4C16-803C-CC86B39579AB}" name="Casa" dataDxfId="16"/>
+    <tableColumn id="3" xr3:uid="{635A1EAB-821A-4F26-9065-6FB417518A06}" name="Visitante" dataDxfId="15"/>
+    <tableColumn id="4" xr3:uid="{FBE8146B-C7EC-4C50-B019-1EA1BA1BF381}" name="Programa" dataDxfId="14"/>
+    <tableColumn id="5" xr3:uid="{39A7C7D3-ADD2-468E-A2C2-BCC114E3E9AA}" name="Final" dataDxfId="13"/>
+    <tableColumn id="6" xr3:uid="{FDB540FF-D930-46F9-BFEA-73BA9AC35CE9}" name="Observaciones" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F524C6FB-FD12-4543-91E2-0257BE7098DE}" name="Tabla547" displayName="Tabla547" ref="H1:I6" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{F524C6FB-FD12-4543-91E2-0257BE7098DE}" name="Tabla547" displayName="Tabla547" ref="H1:I6" totalsRowShown="0" headerRowDxfId="11" dataDxfId="10">
   <autoFilter ref="H1:I6" xr:uid="{60AA24C5-54DC-462B-8486-C4D0E7EF0011}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{55741CEC-D872-49F7-A581-C18D526F204A}" name="Observación" dataDxfId="13"/>
-    <tableColumn id="2" xr3:uid="{4DD9F8EC-0FC2-44EC-A09E-3B34DC2AEA99}" name="Descripción" dataDxfId="12"/>
+    <tableColumn id="1" xr3:uid="{55741CEC-D872-49F7-A581-C18D526F204A}" name="Observación" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{4DD9F8EC-0FC2-44EC-A09E-3B34DC2AEA99}" name="Descripción" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1718,8 +1681,8 @@
   <sheetPr codeName="Hoja1"/>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F13" sqref="F11:F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1950,60 +1913,122 @@
       </c>
     </row>
     <row r="11" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="3"/>
+      <c r="A11" s="2">
+        <v>45365</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="12" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="3"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="3"/>
+      <c r="A12" s="2">
+        <v>45365</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="13" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="3"/>
+      <c r="A13" s="2">
+        <v>45365</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="14" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="4"/>
+      <c r="A14" s="2">
+        <v>45365</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
+      <c r="A15" s="2">
+        <v>45365</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E15" s="4"/>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="3"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="3"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="3"/>
+      <c r="A16" s="6">
+        <v>45365</v>
+      </c>
+      <c r="B16" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D16" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="8"/>
+      <c r="F16" s="7"/>
     </row>
     <row r="17" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A17" s="6"/>
-      <c r="B17" s="7"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="7"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="7"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+      <c r="E17" s="4"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A18" s="2"/>
@@ -2081,12 +2106,20 @@
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E3:E26">
-    <cfRule type="cellIs" dxfId="9" priority="2" operator="equal">
+  <conditionalFormatting sqref="E3:E10 E15:E26">
+    <cfRule type="cellIs" dxfId="7" priority="4" operator="equal">
       <formula>$D3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="8" priority="3" operator="notEqual">
+    <cfRule type="cellIs" dxfId="6" priority="5" operator="notEqual">
       <formula>$D3</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11:E14">
+    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+      <formula>$D11</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
+      <formula>$D11</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2103,8 +2136,8 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:I26"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2483,52 +2516,114 @@
       <c r="F18" s="7"/>
     </row>
     <row r="19" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="3"/>
+      <c r="A19" s="2">
+        <v>45365</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="20" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="3"/>
+      <c r="A20" s="2">
+        <v>45365</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="21" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="3"/>
+      <c r="A21" s="2">
+        <v>45365</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F21" s="3" t="s">
+        <v>56</v>
+      </c>
     </row>
     <row r="22" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A22" s="2"/>
-      <c r="B22" s="3"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="4"/>
+      <c r="A22" s="2">
+        <v>45365</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>14</v>
+      </c>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A23" s="2"/>
-      <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="3"/>
+      <c r="A23" s="2">
+        <v>45365</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>24</v>
+      </c>
       <c r="E23" s="4"/>
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A24" s="2"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="3"/>
+      <c r="A24" s="6">
+        <v>45365</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="D24" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="E24" s="8"/>
+      <c r="F24" s="7"/>
     </row>
     <row r="25" spans="1:6" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A25" s="2"/>
@@ -2550,19 +2645,11 @@
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
   </mergeCells>
-  <conditionalFormatting sqref="E19:E26">
-    <cfRule type="cellIs" dxfId="7" priority="3" operator="equal">
-      <formula>$D19</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="4" operator="notEqual">
-      <formula>$D19</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="E3:E18">
-    <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">
+  <conditionalFormatting sqref="E3:E26">
+    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
       <formula>$D3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="4" priority="2" operator="notEqual">
       <formula>$D3</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2856,10 +2943,10 @@
     <mergeCell ref="A1:F1"/>
   </mergeCells>
   <conditionalFormatting sqref="E3:E26">
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="equal">
       <formula>$D3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="notEqual">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="notEqual">
       <formula>$D3</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>